<commit_message>
Adds standard atmosphere interpolator
</commit_message>
<xml_diff>
--- a/atmosphere.xlsx
+++ b/atmosphere.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18229"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\Jupyter_Notebooks\Aircraft_Performance\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="120" windowWidth="17235" windowHeight="5970"/>
   </bookViews>
@@ -11,12 +16,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>alt</t>
   </si>
@@ -47,14 +52,11 @@
   <si>
     <t>k.visc</t>
   </si>
-  <si>
-    <t>ratio</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -96,6 +98,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -144,7 +149,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -177,9 +182,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -212,6 +234,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -388,15 +427,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K43"/>
+  <dimension ref="A1:J44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -427,894 +466,816 @@
       <c r="J1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>-0.5</v>
-      </c>
-      <c r="B2">
+        <v>-2000</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1.2067000000000001</v>
+      </c>
+      <c r="C2" s="1">
+        <v>1.2611000000000001</v>
+      </c>
+      <c r="D2">
+        <v>1.0450999999999999</v>
+      </c>
+      <c r="E2">
+        <v>301.2</v>
+      </c>
+      <c r="F2" s="1">
+        <v>127800</v>
+      </c>
+      <c r="G2" s="1">
+        <v>1.478</v>
+      </c>
+      <c r="H2">
+        <v>347.9</v>
+      </c>
+      <c r="I2">
+        <v>18.510000000000002</v>
+      </c>
+      <c r="J2" s="1">
+        <v>1.2500000000000001E-5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>-500</v>
+      </c>
+      <c r="B3">
         <v>1.0488999999999999</v>
       </c>
-      <c r="C2">
+      <c r="C3">
         <v>1.0607</v>
       </c>
-      <c r="D2">
+      <c r="D3">
         <v>1.0113000000000001</v>
       </c>
-      <c r="E2">
+      <c r="E3">
         <v>291.39999999999998</v>
       </c>
-      <c r="F2">
+      <c r="F3">
         <v>107477</v>
       </c>
-      <c r="G2">
+      <c r="G3">
         <v>1.2849999999999999</v>
       </c>
-      <c r="H2">
+      <c r="H3">
         <v>342.2</v>
       </c>
-      <c r="I2">
+      <c r="I3">
         <v>18.05</v>
       </c>
-      <c r="J2" s="1">
+      <c r="J3" s="1">
         <v>1.4E-5</v>
       </c>
-      <c r="K2">
-        <v>24.36</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3">
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4">
         <v>0</v>
       </c>
-      <c r="B3">
+      <c r="B4">
         <v>1</v>
       </c>
-      <c r="C3">
+      <c r="C4">
         <v>1</v>
       </c>
-      <c r="D3">
+      <c r="D4">
         <v>1</v>
       </c>
-      <c r="E3">
+      <c r="E4">
         <v>288.10000000000002</v>
       </c>
-      <c r="F3">
+      <c r="F4">
         <v>101325</v>
       </c>
-      <c r="G3">
+      <c r="G4">
         <v>1.2250000000000001</v>
       </c>
-      <c r="H3">
+      <c r="H4">
         <v>340.3</v>
       </c>
-      <c r="I3">
+      <c r="I4">
         <v>17.89</v>
       </c>
-      <c r="J3" s="1">
+      <c r="J4" s="1">
         <v>1.4600000000000001E-5</v>
       </c>
-      <c r="K3">
-        <v>23.3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>0.5</v>
-      </c>
-      <c r="B4">
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>500</v>
+      </c>
+      <c r="B5">
         <v>0.95289999999999997</v>
       </c>
-      <c r="C4">
+      <c r="C5">
         <v>0.94210000000000005</v>
       </c>
-      <c r="D4">
+      <c r="D5">
         <v>0.98870000000000002</v>
       </c>
-      <c r="E4">
+      <c r="E5">
         <v>284.89999999999998</v>
       </c>
-      <c r="F4">
+      <c r="F5">
         <v>95461</v>
       </c>
-      <c r="G4">
+      <c r="G5">
         <v>1.167</v>
       </c>
-      <c r="H4">
+      <c r="H5">
         <v>338.4</v>
       </c>
-      <c r="I4">
+      <c r="I5">
         <v>17.739999999999998</v>
       </c>
-      <c r="J4" s="1">
+      <c r="J5" s="1">
         <v>1.52E-5</v>
       </c>
-      <c r="K4">
-        <v>22.27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>1</v>
-      </c>
-      <c r="B5">
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>1000</v>
+      </c>
+      <c r="B6">
         <v>0.90749999999999997</v>
       </c>
-      <c r="C5">
+      <c r="C6">
         <v>0.88700000000000001</v>
       </c>
-      <c r="D5">
+      <c r="D6">
         <v>0.97740000000000005</v>
       </c>
-      <c r="E5">
+      <c r="E6">
         <v>281.7</v>
       </c>
-      <c r="F5">
+      <c r="F6">
         <v>89876</v>
       </c>
-      <c r="G5">
+      <c r="G6">
         <v>1.1120000000000001</v>
       </c>
-      <c r="H5">
+      <c r="H6">
         <v>336.4</v>
       </c>
-      <c r="I5">
+      <c r="I6">
         <v>17.579999999999998</v>
       </c>
-      <c r="J5" s="1">
+      <c r="J6" s="1">
         <v>1.5800000000000001E-5</v>
       </c>
-      <c r="K5">
-        <v>21.28</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>1.5</v>
-      </c>
-      <c r="B6">
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>1500</v>
+      </c>
+      <c r="B7">
         <v>0.86380000000000001</v>
       </c>
-      <c r="C6">
+      <c r="C7">
         <v>0.83450000000000002</v>
       </c>
-      <c r="D6">
+      <c r="D7">
         <v>0.96619999999999995</v>
       </c>
-      <c r="E6">
+      <c r="E7">
         <v>278.39999999999998</v>
       </c>
-      <c r="F6">
+      <c r="F7">
         <v>84559</v>
       </c>
-      <c r="G6">
+      <c r="G7">
         <v>1.0580000000000001</v>
       </c>
-      <c r="H6">
+      <c r="H7">
         <v>334.5</v>
       </c>
-      <c r="I6">
+      <c r="I7">
         <v>17.420000000000002</v>
       </c>
-      <c r="J6" s="1">
+      <c r="J7" s="1">
         <v>1.6500000000000001E-5</v>
       </c>
-      <c r="K6">
-        <v>20.32</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>2</v>
-      </c>
-      <c r="B7">
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>2000</v>
+      </c>
+      <c r="B8">
         <v>0.82169999999999999</v>
       </c>
-      <c r="C7">
+      <c r="C8">
         <v>0.78459999999999996</v>
       </c>
-      <c r="D7">
+      <c r="D8">
         <v>0.95489999999999997</v>
       </c>
-      <c r="E7">
+      <c r="E8">
         <v>275.2</v>
       </c>
-      <c r="F7">
+      <c r="F8">
         <v>79501</v>
       </c>
-      <c r="G7">
+      <c r="G8">
         <v>1.0069999999999999</v>
       </c>
-      <c r="H7">
+      <c r="H8">
         <v>332.5</v>
       </c>
-      <c r="I7">
+      <c r="I8">
         <v>17.260000000000002</v>
       </c>
-      <c r="J7" s="1">
+      <c r="J8" s="1">
         <v>1.7099999999999999E-5</v>
       </c>
-      <c r="K7">
-        <v>19.39</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>2.5</v>
-      </c>
-      <c r="B8">
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>2500</v>
+      </c>
+      <c r="B9">
         <v>0.78120000000000001</v>
       </c>
-      <c r="C8">
+      <c r="C9">
         <v>0.73719999999999997</v>
       </c>
-      <c r="D8">
+      <c r="D9">
         <v>0.94359999999999999</v>
       </c>
-      <c r="E8">
+      <c r="E9">
         <v>271.89999999999998</v>
       </c>
-      <c r="F8">
+      <c r="F9">
         <v>74691</v>
       </c>
-      <c r="G8">
+      <c r="G9">
         <v>0.95699999999999996</v>
       </c>
-      <c r="H8">
+      <c r="H9">
         <v>330.6</v>
       </c>
-      <c r="I8">
+      <c r="I9">
         <v>17.100000000000001</v>
       </c>
-      <c r="J8" s="1">
+      <c r="J9" s="1">
         <v>1.7900000000000001E-5</v>
       </c>
-      <c r="K8">
-        <v>18.5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>3</v>
-      </c>
-      <c r="B9">
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>3000</v>
+      </c>
+      <c r="B10">
         <v>0.74219999999999997</v>
       </c>
-      <c r="C9">
+      <c r="C10">
         <v>0.69199999999999995</v>
       </c>
-      <c r="D9">
+      <c r="D10">
         <v>0.93240000000000001</v>
       </c>
-      <c r="E9">
+      <c r="E10">
         <v>268.7</v>
       </c>
-      <c r="F9">
+      <c r="F10">
         <v>70121</v>
       </c>
-      <c r="G9">
+      <c r="G10">
         <v>0.90900000000000003</v>
       </c>
-      <c r="H9">
+      <c r="H10">
         <v>328.6</v>
       </c>
-      <c r="I9">
+      <c r="I10">
         <v>16.940000000000001</v>
       </c>
-      <c r="J9" s="1">
+      <c r="J10" s="1">
         <v>1.8600000000000001E-5</v>
       </c>
-      <c r="K9">
-        <v>17.64</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>3.5</v>
-      </c>
-      <c r="B10">
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>3500</v>
+      </c>
+      <c r="B11">
         <v>0.70479999999999998</v>
       </c>
-      <c r="C10">
+      <c r="C11">
         <v>0.6492</v>
       </c>
-      <c r="D10">
+      <c r="D11">
         <v>0.92110000000000003</v>
       </c>
-      <c r="E10">
+      <c r="E11">
         <v>265.39999999999998</v>
       </c>
-      <c r="F10">
+      <c r="F11">
         <v>65780</v>
       </c>
-      <c r="G10">
+      <c r="G11">
         <v>0.86299999999999999</v>
       </c>
-      <c r="H10">
+      <c r="H11">
         <v>326.60000000000002</v>
       </c>
-      <c r="I10">
+      <c r="I11">
         <v>16.78</v>
       </c>
-      <c r="J10" s="1">
+      <c r="J11" s="1">
         <v>1.9400000000000001E-5</v>
       </c>
-      <c r="K10">
-        <v>16.809999999999999</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>4</v>
-      </c>
-      <c r="B11">
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>4000</v>
+      </c>
+      <c r="B12">
         <v>0.66890000000000005</v>
       </c>
-      <c r="C11">
+      <c r="C12">
         <v>0.60850000000000004</v>
       </c>
-      <c r="D11">
+      <c r="D12">
         <v>0.90980000000000005</v>
       </c>
-      <c r="E11">
+      <c r="E12">
         <v>262.2</v>
       </c>
-      <c r="F11">
+      <c r="F12">
         <v>61660</v>
       </c>
-      <c r="G11">
+      <c r="G12">
         <v>0.81899999999999995</v>
       </c>
-      <c r="H11">
+      <c r="H12">
         <v>324.60000000000002</v>
       </c>
-      <c r="I11">
+      <c r="I12">
         <v>16.61</v>
       </c>
-      <c r="J11" s="1">
+      <c r="J12" s="1">
         <v>2.0299999999999999E-5</v>
       </c>
-      <c r="K11">
-        <v>16.010000000000002</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>4.5</v>
-      </c>
-      <c r="B12">
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>4500</v>
+      </c>
+      <c r="B13">
         <v>0.63429999999999997</v>
       </c>
-      <c r="C12">
+      <c r="C13">
         <v>0.56999999999999995</v>
       </c>
-      <c r="D12">
+      <c r="D13">
         <v>0.89859999999999995</v>
       </c>
-      <c r="E12">
+      <c r="E13">
         <v>258.89999999999998</v>
       </c>
-      <c r="F12">
+      <c r="F13">
         <v>57752</v>
       </c>
-      <c r="G12">
+      <c r="G13">
         <v>0.77700000000000002</v>
       </c>
-      <c r="H12">
+      <c r="H13">
         <v>322.60000000000002</v>
       </c>
-      <c r="I12">
+      <c r="I13">
         <v>16.45</v>
       </c>
-      <c r="J12" s="1">
+      <c r="J13" s="1">
         <v>2.12E-5</v>
       </c>
-      <c r="K12">
-        <v>15.24</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>5</v>
-      </c>
-      <c r="B13">
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>5000</v>
+      </c>
+      <c r="B14">
         <v>0.60119999999999996</v>
       </c>
-      <c r="C13">
+      <c r="C14">
         <v>0.53339999999999999</v>
       </c>
-      <c r="D13">
+      <c r="D14">
         <v>0.88729999999999998</v>
       </c>
-      <c r="E13">
+      <c r="E14">
         <v>255.7</v>
       </c>
-      <c r="F13">
+      <c r="F14">
         <v>54048</v>
       </c>
-      <c r="G13">
+      <c r="G14">
         <v>0.73599999999999999</v>
       </c>
-      <c r="H13">
+      <c r="H14">
         <v>320.5</v>
       </c>
-      <c r="I13">
+      <c r="I14">
         <v>16.28</v>
       </c>
-      <c r="J13" s="1">
+      <c r="J14" s="1">
         <v>2.2099999999999998E-5</v>
       </c>
-      <c r="K13">
-        <v>14.5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>5.5</v>
-      </c>
-      <c r="B14">
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>5500</v>
+      </c>
+      <c r="B15">
         <v>0.56940000000000002</v>
       </c>
-      <c r="C14">
+      <c r="C15">
         <v>0.49880000000000002</v>
       </c>
-      <c r="D14">
+      <c r="D15">
         <v>0.876</v>
       </c>
-      <c r="E14">
+      <c r="E15">
         <v>252.4</v>
       </c>
-      <c r="F14">
+      <c r="F15">
         <v>50539</v>
       </c>
-      <c r="G14">
+      <c r="G15">
         <v>0.69699999999999995</v>
       </c>
-      <c r="H14">
+      <c r="H15">
         <v>318.5</v>
       </c>
-      <c r="I14">
+      <c r="I15">
         <v>16.12</v>
       </c>
-      <c r="J14" s="1">
+      <c r="J15" s="1">
         <v>2.3099999999999999E-5</v>
       </c>
-      <c r="K14">
-        <v>13.78</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>6</v>
-      </c>
-      <c r="B15">
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>6000</v>
+      </c>
+      <c r="B16">
         <v>0.53890000000000005</v>
       </c>
-      <c r="C15">
+      <c r="C16">
         <v>0.46600000000000003</v>
       </c>
-      <c r="D15">
+      <c r="D16">
         <v>0.86480000000000001</v>
       </c>
-      <c r="E15">
+      <c r="E16">
         <v>249.2</v>
       </c>
-      <c r="F15">
+      <c r="F16">
         <v>47217</v>
       </c>
-      <c r="G15">
+      <c r="G16">
         <v>0.66</v>
       </c>
-      <c r="H15">
+      <c r="H16">
         <v>316.5</v>
       </c>
-      <c r="I15">
+      <c r="I16">
         <v>15.95</v>
       </c>
-      <c r="J15" s="1">
+      <c r="J16" s="1">
         <v>2.4199999999999999E-5</v>
       </c>
-      <c r="K15">
-        <v>13.1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>6.5</v>
-      </c>
-      <c r="B16">
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>6500</v>
+      </c>
+      <c r="B17">
         <v>0.50960000000000005</v>
       </c>
-      <c r="C16">
+      <c r="C17">
         <v>0.435</v>
       </c>
-      <c r="D16">
+      <c r="D17">
         <v>0.85350000000000004</v>
       </c>
-      <c r="E16">
+      <c r="E17">
         <v>245.9</v>
       </c>
-      <c r="F16">
+      <c r="F17">
         <v>44075</v>
       </c>
-      <c r="G16">
+      <c r="G17">
         <v>0.624</v>
       </c>
-      <c r="H16">
+      <c r="H17">
         <v>314.39999999999998</v>
       </c>
-      <c r="I16">
+      <c r="I17">
         <v>15.78</v>
       </c>
-      <c r="J16" s="1">
+      <c r="J17" s="1">
         <v>2.5299999999999998E-5</v>
       </c>
-      <c r="K16">
-        <v>12.44</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>7</v>
-      </c>
-      <c r="B17">
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>7000</v>
+      </c>
+      <c r="B18">
         <v>0.48159999999999997</v>
       </c>
-      <c r="C17">
+      <c r="C18">
         <v>0.40570000000000001</v>
       </c>
-      <c r="D17">
+      <c r="D18">
         <v>0.84230000000000005</v>
       </c>
-      <c r="E17">
+      <c r="E18">
         <v>242.7</v>
       </c>
-      <c r="F17">
+      <c r="F18">
         <v>41105</v>
       </c>
-      <c r="G17">
+      <c r="G18">
         <v>0.59</v>
       </c>
-      <c r="H17">
+      <c r="H18">
         <v>312.3</v>
       </c>
-      <c r="I17">
+      <c r="I18">
         <v>15.61</v>
       </c>
-      <c r="J17" s="1">
+      <c r="J18" s="1">
         <v>2.65E-5</v>
       </c>
-      <c r="K17">
-        <v>11.8</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>7.5</v>
-      </c>
-      <c r="B18">
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>7500</v>
+      </c>
+      <c r="B19">
         <v>0.45479999999999998</v>
       </c>
-      <c r="C18">
+      <c r="C19">
         <v>0.378</v>
       </c>
-      <c r="D18">
+      <c r="D19">
         <v>0.83099999999999996</v>
       </c>
-      <c r="E18">
+      <c r="E19">
         <v>239.5</v>
       </c>
-      <c r="F18">
+      <c r="F19">
         <v>38299</v>
       </c>
-      <c r="G18">
+      <c r="G19">
         <v>0.55700000000000005</v>
       </c>
-      <c r="H18">
+      <c r="H19">
         <v>310.2</v>
       </c>
-      <c r="I18">
+      <c r="I19">
         <v>15.44</v>
       </c>
-      <c r="J18" s="1">
+      <c r="J19" s="1">
         <v>2.7699999999999999E-5</v>
       </c>
-      <c r="K18">
-        <v>11.19</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>8</v>
-      </c>
-      <c r="B19">
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>8000</v>
+      </c>
+      <c r="B20">
         <v>0.42920000000000003</v>
       </c>
-      <c r="C19">
+      <c r="C20">
         <v>0.35189999999999999</v>
       </c>
-      <c r="D19">
+      <c r="D20">
         <v>0.81979999999999997</v>
       </c>
-      <c r="E19">
+      <c r="E20">
         <v>236.2</v>
       </c>
-      <c r="F19">
+      <c r="F20">
         <v>35651</v>
       </c>
-      <c r="G19">
+      <c r="G20">
         <v>0.52600000000000002</v>
       </c>
-      <c r="H19">
+      <c r="H20">
         <v>308.10000000000002</v>
       </c>
-      <c r="I19">
+      <c r="I20">
         <v>15.27</v>
       </c>
-      <c r="J19" s="1">
+      <c r="J20" s="1">
         <v>2.9E-5</v>
       </c>
-      <c r="K19">
-        <v>10.61</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>8.5</v>
-      </c>
-      <c r="B20">
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>8500</v>
+      </c>
+      <c r="B21">
         <v>0.4047</v>
       </c>
-      <c r="C20">
+      <c r="C21">
         <v>0.32719999999999999</v>
       </c>
-      <c r="D20">
+      <c r="D21">
         <v>0.8085</v>
       </c>
-      <c r="E20">
+      <c r="E21">
         <v>233</v>
       </c>
-      <c r="F20">
+      <c r="F21">
         <v>33154</v>
       </c>
-      <c r="G20">
+      <c r="G21">
         <v>0.496</v>
       </c>
-      <c r="H20">
+      <c r="H21">
         <v>306</v>
       </c>
-      <c r="I20">
+      <c r="I21">
         <v>15.1</v>
       </c>
-      <c r="J20" s="1">
+      <c r="J21" s="1">
         <v>3.0499999999999999E-5</v>
       </c>
-      <c r="K20">
-        <v>10.050000000000001</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>9</v>
-      </c>
-      <c r="B21">
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>9000</v>
+      </c>
+      <c r="B22">
         <v>0.38129999999999997</v>
       </c>
-      <c r="C21">
+      <c r="C22">
         <v>0.30399999999999999</v>
       </c>
-      <c r="D21">
+      <c r="D22">
         <v>0.79730000000000001</v>
       </c>
-      <c r="E21">
+      <c r="E22">
         <v>229.7</v>
       </c>
-      <c r="F21">
+      <c r="F22">
         <v>30800</v>
       </c>
-      <c r="G21">
+      <c r="G22">
         <v>0.46700000000000003</v>
       </c>
-      <c r="H21">
+      <c r="H22">
         <v>303.8</v>
       </c>
-      <c r="I21">
+      <c r="I22">
         <v>14.93</v>
       </c>
-      <c r="J21" s="1">
+      <c r="J22" s="1">
         <v>3.1999999999999999E-5</v>
       </c>
-      <c r="K21">
-        <v>9.51</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>9.5</v>
-      </c>
-      <c r="B22">
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>9500</v>
+      </c>
+      <c r="B23">
         <v>0.3589</v>
       </c>
-      <c r="C22">
+      <c r="C23">
         <v>0.28210000000000002</v>
       </c>
-      <c r="D22">
+      <c r="D23">
         <v>0.78600000000000003</v>
       </c>
-      <c r="E22">
+      <c r="E23">
         <v>226.5</v>
       </c>
-      <c r="F22">
+      <c r="F23">
         <v>28584</v>
       </c>
-      <c r="G22">
+      <c r="G23">
         <v>0.44</v>
       </c>
-      <c r="H22">
+      <c r="H23">
         <v>301.7</v>
       </c>
-      <c r="I22">
+      <c r="I23">
         <v>14.75</v>
       </c>
-      <c r="J22" s="1">
+      <c r="J23" s="1">
         <v>3.3599999999999997E-5</v>
       </c>
-      <c r="K22">
-        <v>8.99</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>10</v>
-      </c>
-      <c r="B23">
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>10000</v>
+      </c>
+      <c r="B24">
         <v>0.33760000000000001</v>
       </c>
-      <c r="C23">
+      <c r="C24">
         <v>0.26150000000000001</v>
       </c>
-      <c r="D23">
+      <c r="D24">
         <v>0.77480000000000004</v>
       </c>
-      <c r="E23">
+      <c r="E24">
         <v>223.3</v>
       </c>
-      <c r="F23">
+      <c r="F24">
         <v>26499</v>
       </c>
-      <c r="G23">
+      <c r="G24">
         <v>0.41399999999999998</v>
       </c>
-      <c r="H23">
+      <c r="H24">
         <v>299.5</v>
       </c>
-      <c r="I23">
+      <c r="I24">
         <v>14.58</v>
       </c>
-      <c r="J23" s="1">
+      <c r="J24" s="1">
         <v>3.5299999999999997E-5</v>
       </c>
-      <c r="K23">
-        <v>8.5</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>10.5</v>
-      </c>
-      <c r="B24">
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>10500</v>
+      </c>
+      <c r="B25">
         <v>0.31719999999999998</v>
       </c>
-      <c r="C24">
+      <c r="C25">
         <v>0.2422</v>
       </c>
-      <c r="D24">
+      <c r="D25">
         <v>0.76349999999999996</v>
       </c>
-      <c r="E24">
+      <c r="E25">
         <v>220</v>
       </c>
-      <c r="F24">
+      <c r="F25">
         <v>24540</v>
       </c>
-      <c r="G24">
+      <c r="G25">
         <v>0.38900000000000001</v>
       </c>
-      <c r="H24">
+      <c r="H25">
         <v>297.39999999999998</v>
       </c>
-      <c r="I24">
+      <c r="I25">
         <v>14.4</v>
       </c>
-      <c r="J24" s="1">
+      <c r="J25" s="1">
         <v>3.7100000000000001E-5</v>
       </c>
-      <c r="K24">
-        <v>8.02</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>11</v>
-      </c>
-      <c r="B25">
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>11000</v>
+      </c>
+      <c r="B26">
         <v>0.29780000000000001</v>
       </c>
-      <c r="C25">
+      <c r="C26">
         <v>0.224</v>
       </c>
-      <c r="D25">
+      <c r="D26">
         <v>0.75229999999999997</v>
       </c>
-      <c r="E25">
+      <c r="E26">
         <v>216.8</v>
       </c>
-      <c r="F25">
+      <c r="F26">
         <v>22699</v>
       </c>
-      <c r="G25">
+      <c r="G26">
         <v>0.36499999999999999</v>
       </c>
-      <c r="H25">
+      <c r="H26">
         <v>295.2</v>
-      </c>
-      <c r="I25">
-        <v>14.22</v>
-      </c>
-      <c r="J25" s="1">
-        <v>3.8999999999999999E-5</v>
-      </c>
-      <c r="K25">
-        <v>7.57</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>11.5</v>
-      </c>
-      <c r="B26">
-        <v>0.27550000000000002</v>
-      </c>
-      <c r="C26">
-        <v>0.20710000000000001</v>
-      </c>
-      <c r="D26">
-        <v>0.75190000000000001</v>
-      </c>
-      <c r="E26">
-        <v>216.6</v>
-      </c>
-      <c r="F26">
-        <v>20984</v>
-      </c>
-      <c r="G26">
-        <v>0.33700000000000002</v>
-      </c>
-      <c r="H26">
-        <v>295.10000000000002</v>
       </c>
       <c r="I26">
         <v>14.22</v>
       </c>
       <c r="J26" s="1">
-        <v>4.21E-5</v>
-      </c>
-      <c r="K26">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+        <v>3.8999999999999999E-5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>12</v>
+        <v>11500</v>
       </c>
       <c r="B27">
-        <v>0.25459999999999999</v>
+        <v>0.27550000000000002</v>
       </c>
       <c r="C27">
-        <v>0.1915</v>
+        <v>0.20710000000000001</v>
       </c>
       <c r="D27">
         <v>0.75190000000000001</v>
@@ -1323,10 +1284,10 @@
         <v>216.6</v>
       </c>
       <c r="F27">
-        <v>19399</v>
+        <v>20984</v>
       </c>
       <c r="G27">
-        <v>0.312</v>
+        <v>0.33700000000000002</v>
       </c>
       <c r="H27">
         <v>295.10000000000002</v>
@@ -1335,21 +1296,18 @@
         <v>14.22</v>
       </c>
       <c r="J27" s="1">
-        <v>4.5599999999999997E-5</v>
-      </c>
-      <c r="K27">
-        <v>6.47</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+        <v>4.21E-5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>12.5</v>
+        <v>12000</v>
       </c>
       <c r="B28">
-        <v>0.2354</v>
+        <v>0.25459999999999999</v>
       </c>
       <c r="C28">
-        <v>0.17699999999999999</v>
+        <v>0.1915</v>
       </c>
       <c r="D28">
         <v>0.75190000000000001</v>
@@ -1358,10 +1316,10 @@
         <v>216.6</v>
       </c>
       <c r="F28">
-        <v>17933</v>
+        <v>19399</v>
       </c>
       <c r="G28">
-        <v>0.28799999999999998</v>
+        <v>0.312</v>
       </c>
       <c r="H28">
         <v>295.10000000000002</v>
@@ -1370,21 +1328,18 @@
         <v>14.22</v>
       </c>
       <c r="J28" s="1">
-        <v>4.9299999999999999E-5</v>
-      </c>
-      <c r="K28">
-        <v>5.99</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+        <v>4.5599999999999997E-5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>13</v>
+        <v>12500</v>
       </c>
       <c r="B29">
-        <v>0.21759999999999999</v>
+        <v>0.2354</v>
       </c>
       <c r="C29">
-        <v>0.1636</v>
+        <v>0.17699999999999999</v>
       </c>
       <c r="D29">
         <v>0.75190000000000001</v>
@@ -1393,10 +1348,10 @@
         <v>216.6</v>
       </c>
       <c r="F29">
-        <v>16579</v>
+        <v>17933</v>
       </c>
       <c r="G29">
-        <v>0.26700000000000002</v>
+        <v>0.28799999999999998</v>
       </c>
       <c r="H29">
         <v>295.10000000000002</v>
@@ -1405,21 +1360,18 @@
         <v>14.22</v>
       </c>
       <c r="J29" s="1">
-        <v>5.3300000000000001E-5</v>
-      </c>
-      <c r="K29">
-        <v>5.53</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+        <v>4.9299999999999999E-5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>13.5</v>
+        <v>13000</v>
       </c>
       <c r="B30">
-        <v>0.20119999999999999</v>
+        <v>0.21759999999999999</v>
       </c>
       <c r="C30">
-        <v>0.15129999999999999</v>
+        <v>0.1636</v>
       </c>
       <c r="D30">
         <v>0.75190000000000001</v>
@@ -1428,10 +1380,10 @@
         <v>216.6</v>
       </c>
       <c r="F30">
-        <v>15327</v>
+        <v>16579</v>
       </c>
       <c r="G30">
-        <v>0.246</v>
+        <v>0.26700000000000002</v>
       </c>
       <c r="H30">
         <v>295.10000000000002</v>
@@ -1440,21 +1392,18 @@
         <v>14.22</v>
       </c>
       <c r="J30" s="1">
-        <v>5.77E-5</v>
-      </c>
-      <c r="K30">
-        <v>5.12</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+        <v>5.3300000000000001E-5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>14</v>
+        <v>13500</v>
       </c>
       <c r="B31">
-        <v>0.186</v>
+        <v>0.20119999999999999</v>
       </c>
       <c r="C31">
-        <v>0.13980000000000001</v>
+        <v>0.15129999999999999</v>
       </c>
       <c r="D31">
         <v>0.75190000000000001</v>
@@ -1463,10 +1412,10 @@
         <v>216.6</v>
       </c>
       <c r="F31">
-        <v>14170</v>
+        <v>15327</v>
       </c>
       <c r="G31">
-        <v>0.22800000000000001</v>
+        <v>0.246</v>
       </c>
       <c r="H31">
         <v>295.10000000000002</v>
@@ -1475,21 +1424,18 @@
         <v>14.22</v>
       </c>
       <c r="J31" s="1">
-        <v>6.2399999999999999E-5</v>
-      </c>
-      <c r="K31">
-        <v>4.7300000000000004</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+        <v>5.77E-5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>14.5</v>
+        <v>14000</v>
       </c>
       <c r="B32">
-        <v>0.17199999999999999</v>
+        <v>0.186</v>
       </c>
       <c r="C32">
-        <v>0.1293</v>
+        <v>0.13980000000000001</v>
       </c>
       <c r="D32">
         <v>0.75190000000000001</v>
@@ -1498,10 +1444,10 @@
         <v>216.6</v>
       </c>
       <c r="F32">
-        <v>13100</v>
+        <v>14170</v>
       </c>
       <c r="G32">
-        <v>0.21099999999999999</v>
+        <v>0.22800000000000001</v>
       </c>
       <c r="H32">
         <v>295.10000000000002</v>
@@ -1510,21 +1456,18 @@
         <v>14.22</v>
       </c>
       <c r="J32" s="1">
-        <v>6.7500000000000001E-5</v>
-      </c>
-      <c r="K32">
-        <v>4.37</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+        <v>6.2399999999999999E-5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>15</v>
+        <v>14500</v>
       </c>
       <c r="B33">
-        <v>0.159</v>
+        <v>0.17199999999999999</v>
       </c>
       <c r="C33">
-        <v>0.1195</v>
+        <v>0.1293</v>
       </c>
       <c r="D33">
         <v>0.75190000000000001</v>
@@ -1533,10 +1476,10 @@
         <v>216.6</v>
       </c>
       <c r="F33">
-        <v>12111</v>
+        <v>13100</v>
       </c>
       <c r="G33">
-        <v>0.19500000000000001</v>
+        <v>0.21099999999999999</v>
       </c>
       <c r="H33">
         <v>295.10000000000002</v>
@@ -1545,21 +1488,18 @@
         <v>14.22</v>
       </c>
       <c r="J33" s="1">
-        <v>7.2999999999999999E-5</v>
-      </c>
-      <c r="K33">
-        <v>4.04</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+        <v>6.7500000000000001E-5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>15.5</v>
+        <v>15000</v>
       </c>
       <c r="B34">
-        <v>0.14699999999999999</v>
+        <v>0.159</v>
       </c>
       <c r="C34">
-        <v>0.1105</v>
+        <v>0.1195</v>
       </c>
       <c r="D34">
         <v>0.75190000000000001</v>
@@ -1568,10 +1508,10 @@
         <v>216.6</v>
       </c>
       <c r="F34">
-        <v>11197</v>
+        <v>12111</v>
       </c>
       <c r="G34">
-        <v>0.18</v>
+        <v>0.19500000000000001</v>
       </c>
       <c r="H34">
         <v>295.10000000000002</v>
@@ -1580,21 +1520,18 @@
         <v>14.22</v>
       </c>
       <c r="J34" s="1">
-        <v>7.8999999999999996E-5</v>
-      </c>
-      <c r="K34">
-        <v>3.74</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+        <v>7.2999999999999999E-5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>16</v>
+        <v>15500</v>
       </c>
       <c r="B35">
-        <v>0.13589999999999999</v>
+        <v>0.14699999999999999</v>
       </c>
       <c r="C35">
-        <v>0.1022</v>
+        <v>0.1105</v>
       </c>
       <c r="D35">
         <v>0.75190000000000001</v>
@@ -1603,10 +1540,10 @@
         <v>216.6</v>
       </c>
       <c r="F35">
-        <v>10352</v>
+        <v>11197</v>
       </c>
       <c r="G35">
-        <v>0.16600000000000001</v>
+        <v>0.18</v>
       </c>
       <c r="H35">
         <v>295.10000000000002</v>
@@ -1615,21 +1552,18 @@
         <v>14.22</v>
       </c>
       <c r="J35" s="1">
-        <v>8.5400000000000002E-5</v>
-      </c>
-      <c r="K35">
-        <v>3.46</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+        <v>7.8999999999999996E-5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>16.5</v>
+        <v>16000</v>
       </c>
       <c r="B36">
-        <v>0.12559999999999999</v>
+        <v>0.13589999999999999</v>
       </c>
       <c r="C36">
-        <v>9.4500000000000001E-2</v>
+        <v>0.1022</v>
       </c>
       <c r="D36">
         <v>0.75190000000000001</v>
@@ -1638,10 +1572,10 @@
         <v>216.6</v>
       </c>
       <c r="F36">
-        <v>9571</v>
+        <v>10352</v>
       </c>
       <c r="G36">
-        <v>0.154</v>
+        <v>0.16600000000000001</v>
       </c>
       <c r="H36">
         <v>295.10000000000002</v>
@@ -1650,21 +1584,18 @@
         <v>14.22</v>
       </c>
       <c r="J36" s="1">
-        <v>9.2399999999999996E-5</v>
-      </c>
-      <c r="K36">
-        <v>3.19</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+        <v>8.5400000000000002E-5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>17</v>
+        <v>16500</v>
       </c>
       <c r="B37">
-        <v>0.1162</v>
+        <v>0.12559999999999999</v>
       </c>
       <c r="C37">
-        <v>8.7300000000000003E-2</v>
+        <v>9.4500000000000001E-2</v>
       </c>
       <c r="D37">
         <v>0.75190000000000001</v>
@@ -1673,10 +1604,10 @@
         <v>216.6</v>
       </c>
       <c r="F37">
-        <v>8849</v>
+        <v>9571</v>
       </c>
       <c r="G37">
-        <v>0.14199999999999999</v>
+        <v>0.154</v>
       </c>
       <c r="H37">
         <v>295.10000000000002</v>
@@ -1685,21 +1616,18 @@
         <v>14.22</v>
       </c>
       <c r="J37" s="1">
-        <v>9.9900000000000002E-5</v>
-      </c>
-      <c r="K37">
-        <v>2.95</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+        <v>9.2399999999999996E-5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>17.5</v>
+        <v>17000</v>
       </c>
       <c r="B38">
-        <v>0.1074</v>
+        <v>0.1162</v>
       </c>
       <c r="C38">
-        <v>8.0799999999999997E-2</v>
+        <v>8.7300000000000003E-2</v>
       </c>
       <c r="D38">
         <v>0.75190000000000001</v>
@@ -1708,10 +1636,10 @@
         <v>216.6</v>
       </c>
       <c r="F38">
-        <v>8182</v>
+        <v>8849</v>
       </c>
       <c r="G38">
-        <v>0.13200000000000001</v>
+        <v>0.14199999999999999</v>
       </c>
       <c r="H38">
         <v>295.10000000000002</v>
@@ -1720,21 +1648,18 @@
         <v>14.22</v>
       </c>
       <c r="J38" s="1">
-        <v>1.08E-4</v>
-      </c>
-      <c r="K38">
-        <v>2.73</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+        <v>9.9900000000000002E-5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>18</v>
+        <v>17500</v>
       </c>
       <c r="B39">
-        <v>9.9299999999999999E-2</v>
+        <v>0.1074</v>
       </c>
       <c r="C39">
-        <v>7.4700000000000003E-2</v>
+        <v>8.0799999999999997E-2</v>
       </c>
       <c r="D39">
         <v>0.75190000000000001</v>
@@ -1743,10 +1668,10 @@
         <v>216.6</v>
       </c>
       <c r="F39">
-        <v>7565</v>
+        <v>8182</v>
       </c>
       <c r="G39">
-        <v>0.122</v>
+        <v>0.13200000000000001</v>
       </c>
       <c r="H39">
         <v>295.10000000000002</v>
@@ -1755,21 +1680,18 @@
         <v>14.22</v>
       </c>
       <c r="J39" s="1">
-        <v>1.17E-4</v>
-      </c>
-      <c r="K39">
-        <v>2.52</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+        <v>1.08E-4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>18.5</v>
+        <v>18000</v>
       </c>
       <c r="B40">
-        <v>9.1800000000000007E-2</v>
+        <v>9.9299999999999999E-2</v>
       </c>
       <c r="C40">
-        <v>6.9000000000000006E-2</v>
+        <v>7.4700000000000003E-2</v>
       </c>
       <c r="D40">
         <v>0.75190000000000001</v>
@@ -1778,10 +1700,10 @@
         <v>216.6</v>
       </c>
       <c r="F40">
-        <v>6994</v>
+        <v>7565</v>
       </c>
       <c r="G40">
-        <v>0.112</v>
+        <v>0.122</v>
       </c>
       <c r="H40">
         <v>295.10000000000002</v>
@@ -1790,21 +1712,18 @@
         <v>14.22</v>
       </c>
       <c r="J40" s="1">
-        <v>1.26E-4</v>
-      </c>
-      <c r="K40">
-        <v>2.33</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+        <v>1.17E-4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>19</v>
+        <v>18500</v>
       </c>
       <c r="B41">
-        <v>8.4900000000000003E-2</v>
+        <v>9.1800000000000007E-2</v>
       </c>
       <c r="C41">
-        <v>6.3799999999999996E-2</v>
+        <v>6.9000000000000006E-2</v>
       </c>
       <c r="D41">
         <v>0.75190000000000001</v>
@@ -1813,10 +1732,10 @@
         <v>216.6</v>
       </c>
       <c r="F41">
-        <v>6467</v>
+        <v>6994</v>
       </c>
       <c r="G41">
-        <v>0.104</v>
+        <v>0.112</v>
       </c>
       <c r="H41">
         <v>295.10000000000002</v>
@@ -1825,21 +1744,18 @@
         <v>14.22</v>
       </c>
       <c r="J41" s="1">
-        <v>1.37E-4</v>
-      </c>
-      <c r="K41">
-        <v>2.16</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+        <v>1.26E-4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>19.5</v>
+        <v>19000</v>
       </c>
       <c r="B42">
-        <v>7.85E-2</v>
+        <v>8.4900000000000003E-2</v>
       </c>
       <c r="C42">
-        <v>5.8999999999999997E-2</v>
+        <v>6.3799999999999996E-2</v>
       </c>
       <c r="D42">
         <v>0.75190000000000001</v>
@@ -1848,10 +1764,10 @@
         <v>216.6</v>
       </c>
       <c r="F42">
-        <v>5979</v>
+        <v>6467</v>
       </c>
       <c r="G42">
-        <v>9.6000000000000002E-2</v>
+        <v>0.104</v>
       </c>
       <c r="H42">
         <v>295.10000000000002</v>
@@ -1860,21 +1776,18 @@
         <v>14.22</v>
       </c>
       <c r="J42" s="1">
-        <v>1.4799999999999999E-4</v>
-      </c>
-      <c r="K42">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+        <v>1.37E-4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>20</v>
+        <v>19500</v>
       </c>
       <c r="B43">
-        <v>7.2599999999999998E-2</v>
+        <v>7.85E-2</v>
       </c>
       <c r="C43">
-        <v>5.4600000000000003E-2</v>
+        <v>5.8999999999999997E-2</v>
       </c>
       <c r="D43">
         <v>0.75190000000000001</v>
@@ -1883,10 +1796,10 @@
         <v>216.6</v>
       </c>
       <c r="F43">
-        <v>5529</v>
+        <v>5979</v>
       </c>
       <c r="G43">
-        <v>8.8999999999999996E-2</v>
+        <v>9.6000000000000002E-2</v>
       </c>
       <c r="H43">
         <v>295.10000000000002</v>
@@ -1895,10 +1808,39 @@
         <v>14.22</v>
       </c>
       <c r="J43" s="1">
+        <v>1.4799999999999999E-4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>20000</v>
+      </c>
+      <c r="B44">
+        <v>7.2599999999999998E-2</v>
+      </c>
+      <c r="C44">
+        <v>5.4600000000000003E-2</v>
+      </c>
+      <c r="D44">
+        <v>0.75190000000000001</v>
+      </c>
+      <c r="E44">
+        <v>216.6</v>
+      </c>
+      <c r="F44">
+        <v>5529</v>
+      </c>
+      <c r="G44">
+        <v>8.8999999999999996E-2</v>
+      </c>
+      <c r="H44">
+        <v>295.10000000000002</v>
+      </c>
+      <c r="I44">
+        <v>14.22</v>
+      </c>
+      <c r="J44" s="1">
         <v>1.6000000000000001E-4</v>
-      </c>
-      <c r="K43">
-        <v>1.85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>